<commit_message>
cambios testing Gestion Personas
</commit_message>
<xml_diff>
--- a/Documentacion/Testing/1-MEC_TestingHito1.xlsx
+++ b/Documentacion/Testing/1-MEC_TestingHito1.xlsx
@@ -507,7 +507,7 @@
     <cellStyle name="Incorrecto" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="236">
+  <dxfs count="112">
     <dxf>
       <fill>
         <patternFill>
@@ -525,6 +525,48 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFE0A5A4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEA5A2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="3" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -560,6 +602,41 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFDEA5A2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFE0A5A4"/>
         </patternFill>
       </fill>
@@ -602,6 +679,41 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0A5A4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFDEA5A2"/>
         </patternFill>
       </fill>
@@ -637,6 +749,48 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFE0A5A4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEA5A2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="3" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -672,6 +826,41 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFDEA5A2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFE0A5A4"/>
         </patternFill>
       </fill>
@@ -714,6 +903,41 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0A5A4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFDEA5A2"/>
         </patternFill>
       </fill>
@@ -820,1098 +1044,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0A5A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0A5A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0A5A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0A5A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0A5A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0A5A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0A5A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0A5A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0A5A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0A5A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0A5A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0A5A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0A5A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0A5A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0A5A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0A5A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0A5A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEA5A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2469,12 +1601,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="D93" sqref="D92:D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="77.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
@@ -4646,7 +3779,7 @@
         <v>45622</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -4670,7 +3803,7 @@
         <v>45622</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="30">
@@ -4694,7 +3827,7 @@
         <v>45622</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="30">
@@ -4718,7 +3851,7 @@
         <v>45622</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -4742,7 +3875,7 @@
         <v>45622</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="30">
@@ -4766,7 +3899,7 @@
         <v>45622</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="45">
@@ -4790,427 +3923,427 @@
         <v>45622</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4:D67 D69:D75">
-    <cfRule type="containsText" dxfId="127" priority="398" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="111" priority="398" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="399" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="110" priority="399" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="125" priority="400" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="109" priority="400" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E67 E69:E75">
-    <cfRule type="containsText" dxfId="124" priority="392" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="108" priority="392" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="393" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="107" priority="393" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="394" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="106" priority="394" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H67 H69:H75">
-    <cfRule type="containsText" dxfId="121" priority="387" operator="containsText" text="RESUELTO">
+    <cfRule type="containsText" dxfId="105" priority="387" operator="containsText" text="RESUELTO">
       <formula>NOT(ISERROR(SEARCH("RESUELTO",H4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="388" operator="containsText" text="ABIERTO">
+    <cfRule type="containsText" dxfId="104" priority="388" operator="containsText" text="ABIERTO">
       <formula>NOT(ISERROR(SEARCH("ABIERTO",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D76:D80">
-    <cfRule type="containsText" dxfId="119" priority="102" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="103" priority="102" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",D76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="103" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="102" priority="103" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",D76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="104" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="101" priority="104" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",D76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76:E80">
-    <cfRule type="containsText" dxfId="116" priority="99" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="100" priority="99" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",E76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="100" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="99" priority="100" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",E76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="101" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="98" priority="101" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",E76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H76:H80">
-    <cfRule type="containsText" dxfId="113" priority="97" operator="containsText" text="RESUELTO">
+    <cfRule type="containsText" dxfId="97" priority="97" operator="containsText" text="RESUELTO">
       <formula>NOT(ISERROR(SEARCH("RESUELTO",H76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="98" operator="containsText" text="ABIERTO">
+    <cfRule type="containsText" dxfId="96" priority="98" operator="containsText" text="ABIERTO">
       <formula>NOT(ISERROR(SEARCH("ABIERTO",H76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81">
-    <cfRule type="containsText" dxfId="111" priority="94" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="95" priority="94" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",D81)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="95" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="94" priority="95" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",D81)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="96" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="93" priority="96" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",D81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81">
-    <cfRule type="containsText" dxfId="108" priority="91" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="92" priority="91" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",E81)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="92" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="91" priority="92" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",E81)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="93" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="90" priority="93" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",E81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81">
-    <cfRule type="containsText" dxfId="105" priority="89" operator="containsText" text="RESUELTO">
+    <cfRule type="containsText" dxfId="89" priority="89" operator="containsText" text="RESUELTO">
       <formula>NOT(ISERROR(SEARCH("RESUELTO",H81)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="90" operator="containsText" text="ABIERTO">
+    <cfRule type="containsText" dxfId="88" priority="90" operator="containsText" text="ABIERTO">
       <formula>NOT(ISERROR(SEARCH("ABIERTO",H81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D82">
-    <cfRule type="containsText" dxfId="103" priority="86" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="87" priority="86" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",D82)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="87" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="86" priority="87" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",D82)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="88" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="85" priority="88" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",D82)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E82">
-    <cfRule type="containsText" dxfId="100" priority="83" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="84" priority="83" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",E82)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="84" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="83" priority="84" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",E82)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="85" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="82" priority="85" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",E82)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H82">
-    <cfRule type="containsText" dxfId="97" priority="81" operator="containsText" text="RESUELTO">
+    <cfRule type="containsText" dxfId="81" priority="81" operator="containsText" text="RESUELTO">
       <formula>NOT(ISERROR(SEARCH("RESUELTO",H82)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="82" operator="containsText" text="ABIERTO">
+    <cfRule type="containsText" dxfId="80" priority="82" operator="containsText" text="ABIERTO">
       <formula>NOT(ISERROR(SEARCH("ABIERTO",H82)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D83">
-    <cfRule type="containsText" dxfId="95" priority="78" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="79" priority="78" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",D83)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="79" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="78" priority="79" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",D83)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="80" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="77" priority="80" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",D83)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E83">
-    <cfRule type="containsText" dxfId="92" priority="75" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="76" priority="75" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",E83)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="76" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="75" priority="76" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",E83)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="77" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="74" priority="77" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",E83)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83">
-    <cfRule type="containsText" dxfId="89" priority="73" operator="containsText" text="RESUELTO">
+    <cfRule type="containsText" dxfId="73" priority="73" operator="containsText" text="RESUELTO">
       <formula>NOT(ISERROR(SEARCH("RESUELTO",H83)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="74" operator="containsText" text="ABIERTO">
+    <cfRule type="containsText" dxfId="72" priority="74" operator="containsText" text="ABIERTO">
       <formula>NOT(ISERROR(SEARCH("ABIERTO",H83)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D83">
-    <cfRule type="containsText" dxfId="87" priority="70" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="71" priority="70" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",D83)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="71" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",D83)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="72" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="69" priority="72" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",D83)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E83">
-    <cfRule type="containsText" dxfId="84" priority="67" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="68" priority="67" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",E83)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="68" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",E83)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="69" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="66" priority="69" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",E83)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83">
-    <cfRule type="containsText" dxfId="81" priority="65" operator="containsText" text="RESUELTO">
+    <cfRule type="containsText" dxfId="65" priority="65" operator="containsText" text="RESUELTO">
       <formula>NOT(ISERROR(SEARCH("RESUELTO",H83)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="66" operator="containsText" text="ABIERTO">
+    <cfRule type="containsText" dxfId="64" priority="66" operator="containsText" text="ABIERTO">
       <formula>NOT(ISERROR(SEARCH("ABIERTO",H83)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D86">
-    <cfRule type="containsText" dxfId="79" priority="62" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="63" priority="62" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",D86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="63" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="62" priority="63" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",D86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="64" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="61" priority="64" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",D86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E86">
-    <cfRule type="containsText" dxfId="76" priority="59" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="60" priority="59" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",E86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="60" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="59" priority="60" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",E86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="61" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="58" priority="61" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",E86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H86">
-    <cfRule type="containsText" dxfId="73" priority="57" operator="containsText" text="RESUELTO">
+    <cfRule type="containsText" dxfId="57" priority="57" operator="containsText" text="RESUELTO">
       <formula>NOT(ISERROR(SEARCH("RESUELTO",H86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="58" operator="containsText" text="ABIERTO">
+    <cfRule type="containsText" dxfId="56" priority="58" operator="containsText" text="ABIERTO">
       <formula>NOT(ISERROR(SEARCH("ABIERTO",H86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D87">
-    <cfRule type="containsText" dxfId="71" priority="54" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="55" priority="54" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",D87)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="55" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="54" priority="55" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",D87)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="56" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="53" priority="56" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",D87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="containsText" dxfId="68" priority="51" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="52" priority="51" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",E87)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="52" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="51" priority="52" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",E87)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="53" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="50" priority="53" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",E87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H87">
-    <cfRule type="containsText" dxfId="65" priority="49" operator="containsText" text="RESUELTO">
+    <cfRule type="containsText" dxfId="49" priority="49" operator="containsText" text="RESUELTO">
       <formula>NOT(ISERROR(SEARCH("RESUELTO",H87)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="50" operator="containsText" text="ABIERTO">
+    <cfRule type="containsText" dxfId="48" priority="50" operator="containsText" text="ABIERTO">
       <formula>NOT(ISERROR(SEARCH("ABIERTO",H87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D84">
-    <cfRule type="containsText" dxfId="63" priority="46" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="47" priority="46" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",D84)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="47" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",D84)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="48" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",D84)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E84">
-    <cfRule type="containsText" dxfId="60" priority="43" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",E84)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="44" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",E84)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="45" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="42" priority="45" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",E84)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H84">
-    <cfRule type="containsText" dxfId="57" priority="41" operator="containsText" text="RESUELTO">
+    <cfRule type="containsText" dxfId="41" priority="41" operator="containsText" text="RESUELTO">
       <formula>NOT(ISERROR(SEARCH("RESUELTO",H84)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="42" operator="containsText" text="ABIERTO">
+    <cfRule type="containsText" dxfId="40" priority="42" operator="containsText" text="ABIERTO">
       <formula>NOT(ISERROR(SEARCH("ABIERTO",H84)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="containsText" dxfId="55" priority="38" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="39" priority="38" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",D85)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="39" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="38" priority="39" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",D85)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="40" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="37" priority="40" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",D85)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85">
-    <cfRule type="containsText" dxfId="52" priority="35" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="36" priority="35" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",E85)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="36" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="35" priority="36" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",E85)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="37" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="34" priority="37" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",E85)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H85">
-    <cfRule type="containsText" dxfId="49" priority="33" operator="containsText" text="RESUELTO">
+    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="RESUELTO">
       <formula>NOT(ISERROR(SEARCH("RESUELTO",H85)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="34" operator="containsText" text="ABIERTO">
+    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="ABIERTO">
       <formula>NOT(ISERROR(SEARCH("ABIERTO",H85)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D89">
-    <cfRule type="containsText" dxfId="47" priority="30" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="31" priority="30" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",D89)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="31" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="30" priority="31" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",D89)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="32" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="29" priority="32" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",D89)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E89">
-    <cfRule type="containsText" dxfId="44" priority="27" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="28" priority="27" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",E89)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="28" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",E89)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="29" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",E89)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H89">
-    <cfRule type="containsText" dxfId="41" priority="25" operator="containsText" text="RESUELTO">
+    <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="RESUELTO">
       <formula>NOT(ISERROR(SEARCH("RESUELTO",H89)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="26" operator="containsText" text="ABIERTO">
+    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="ABIERTO">
       <formula>NOT(ISERROR(SEARCH("ABIERTO",H89)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88">
-    <cfRule type="containsText" dxfId="39" priority="22" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",D88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="23" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",D88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="24" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",D88)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E88">
-    <cfRule type="containsText" dxfId="36" priority="19" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",E88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="20" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",E88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="21" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",E88)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H88">
-    <cfRule type="containsText" dxfId="33" priority="17" operator="containsText" text="RESUELTO">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="RESUELTO">
       <formula>NOT(ISERROR(SEARCH("RESUELTO",H88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="18" operator="containsText" text="ABIERTO">
+    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="ABIERTO">
       <formula>NOT(ISERROR(SEARCH("ABIERTO",H88)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75">
-    <cfRule type="containsText" dxfId="31" priority="14" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",D75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="15" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",D75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="16" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",D75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E75">
-    <cfRule type="containsText" dxfId="25" priority="11" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",E75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="12" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",E75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",E75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H75">
-    <cfRule type="containsText" dxfId="19" priority="9" operator="containsText" text="RESUELTO">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="RESUELTO">
       <formula>NOT(ISERROR(SEARCH("RESUELTO",H75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="10" operator="containsText" text="ABIERTO">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="ABIERTO">
       <formula>NOT(ISERROR(SEARCH("ABIERTO",H75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75">
-    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",D75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",D75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",D75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E75">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",E75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",E75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",E75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H75">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="RESUELTO">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="RESUELTO">
       <formula>NOT(ISERROR(SEARCH("RESUELTO",H75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="ABIERTO">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="ABIERTO">
       <formula>NOT(ISERROR(SEARCH("ABIERTO",H75)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>